<commit_message>
Added lunch and dinner menus with the required queries
</commit_message>
<xml_diff>
--- a/src/assets/menu/menu.xlsx
+++ b/src/assets/menu/menu.xlsx
@@ -5,6 +5,8 @@
   <sheets>
     <sheet state="visible" name="Dishes" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Categories" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="LunchAll" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DinnerAll" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="427">
   <si>
     <t>order</t>
   </si>
@@ -887,6 +889,12 @@
     <t>Fried salmon and avocado topped with spicy salmon and spicy mayo</t>
   </si>
   <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
     <t>2 pieces per order</t>
   </si>
   <si>
@@ -906,6 +914,387 @@
   </si>
   <si>
     <t>Udon (soup), Yaki Udon (stir-fried), or Yaki Soba (stir-fried)</t>
+  </si>
+  <si>
+    <t>Soups</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Appetizers</t>
+  </si>
+  <si>
+    <t>Premium Appetizers</t>
+  </si>
+  <si>
+    <t>Nigiri</t>
+  </si>
+  <si>
+    <t>Premium Nigiri</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Premium Roll</t>
+  </si>
+  <si>
+    <t>Soups and Salad</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>Additional Appetizers</t>
+  </si>
+  <si>
+    <t>Additional Nigiri</t>
+  </si>
+  <si>
+    <t>Rolls</t>
+  </si>
+  <si>
+    <t>Additional Rolls</t>
+  </si>
+  <si>
+    <t>spicy</t>
+  </si>
+  <si>
+    <t>Homemade Gyoza (3)</t>
+  </si>
+  <si>
+    <t>Vegetable Tempura (4)</t>
+  </si>
+  <si>
+    <t>Crab Rangoon (2)</t>
+  </si>
+  <si>
+    <t>Edemane</t>
+  </si>
+  <si>
+    <t>Spring Roll</t>
+  </si>
+  <si>
+    <t>General Tso’s Chicken</t>
+  </si>
+  <si>
+    <t>Shumai (3)</t>
+  </si>
+  <si>
+    <t>Avodaco</t>
+  </si>
+  <si>
+    <t>Eel</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Sweet Potato</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Salmon, cream cheese, and scallions. Can be fried or not fried,</t>
+  </si>
+  <si>
+    <t>Cucumber, avocado, masago, and shrimp tempura</t>
+  </si>
+  <si>
+    <t>Tuna, spicy mayo, and crunch</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Salmon, avocado, and cucumber</t>
+  </si>
+  <si>
+    <t>Pickled Radish</t>
+  </si>
+  <si>
+    <t>Cream Cheese</t>
+  </si>
+  <si>
+    <t>Cream cheese and crab.</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>Cream cheese, crab, honey, and crunch</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Futo Maki</t>
+  </si>
+  <si>
+    <t>Cucumber, crab meat, egg, pickled radish, and masago</t>
+  </si>
+  <si>
+    <t>Cucumber, fried sweet potato, and avocado</t>
+  </si>
+  <si>
+    <t>Salmon Skin</t>
+  </si>
+  <si>
+    <t>Spicy Crab</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Fried roll with red snapper, honey, cream cheese, and crab meat</t>
+  </si>
+  <si>
+    <t>Spicy California</t>
+  </si>
+  <si>
+    <t>Jalapeno</t>
+  </si>
+  <si>
+    <t>Cucumber, avocado, crab meat, and jalapeños with spicy mayo</t>
+  </si>
+  <si>
+    <t>Sunset Tokyo</t>
+  </si>
+  <si>
+    <t>Spicy salmon and cucumber with crunch inside and salmon on top</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Lettuce, cucumber, and tempura shrimp</t>
+  </si>
+  <si>
+    <t>Kirin Bomb</t>
+  </si>
+  <si>
+    <t>Fried roll with egg, avocado, and crab meat</t>
+  </si>
+  <si>
+    <t>Crab Meat Tempura</t>
+  </si>
+  <si>
+    <t>Fried roll with jalapeños, crab meat, and cream cheese</t>
+  </si>
+  <si>
+    <t>Crazy Crab</t>
+  </si>
+  <si>
+    <t>Crab meat, cucumber, and avocado topped with spicy crab</t>
+  </si>
+  <si>
+    <t>St. Louis</t>
+  </si>
+  <si>
+    <t>Fried roll with salmon, honey, cream cheese, and crab meat</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>Tuna, avocado, and masago. Can be both fried or not fried.</t>
+  </si>
+  <si>
+    <t>American Dream</t>
+  </si>
+  <si>
+    <t>Shrimp tempura, masago, cucumber, eel, and avocado.</t>
+  </si>
+  <si>
+    <t>Yamasa</t>
+  </si>
+  <si>
+    <t>Crab, masago, and mayo</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Salmon, eel, cucumber, avocado, and masago</t>
+  </si>
+  <si>
+    <t>Crab Salad</t>
+  </si>
+  <si>
+    <t>Chicken Salad</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Sour Chicken</t>
+  </si>
+  <si>
+    <t>Edemame</t>
+  </si>
+  <si>
+    <t>Tempura Oreo (1)</t>
+  </si>
+  <si>
+    <t>Onion Ring</t>
+  </si>
+  <si>
+    <t>Chicken Strips</t>
+  </si>
+  <si>
+    <t>Tempura Squid</t>
+  </si>
+  <si>
+    <t>Tempura Crab Meat</t>
+  </si>
+  <si>
+    <t>Cheese Stick</t>
+  </si>
+  <si>
+    <t>Chicken on Stick</t>
+  </si>
+  <si>
+    <t>Spicy Honey Garlic Chicken</t>
+  </si>
+  <si>
+    <t>Yellowtail</t>
+  </si>
+  <si>
+    <t>Ika Salad</t>
+  </si>
+  <si>
+    <t>Salmon, cream cheese, and scallions</t>
+  </si>
+  <si>
+    <t>Spider</t>
+  </si>
+  <si>
+    <t>Cucumber, avocado, masago, and soft shell crab tempura</t>
+  </si>
+  <si>
+    <t>Shrimp tempura, masago, cucumber, eel, and avocado</t>
+  </si>
+  <si>
+    <t>Either fried or not fried. Tuna, avocado, and masago wrapped inside out</t>
+  </si>
+  <si>
+    <t>Cucumber, avocado, masago, and shrimp</t>
+  </si>
+  <si>
+    <t>Salmon, red snapper, and crab tempura with rice outside</t>
+  </si>
+  <si>
+    <t>Fried roll with salmon, honey cream cheese, and crab meat</t>
+  </si>
+  <si>
+    <t>Sapporo</t>
+  </si>
+  <si>
+    <t>Crab meat, avocado, and cucumber inside with spicy tuna on top</t>
+  </si>
+  <si>
+    <t>Tuna with spicy mayo and crunch</t>
+  </si>
+  <si>
+    <t>Rainbow</t>
+  </si>
+  <si>
+    <t>Crab, cucumber, and avocado with four types of raw fish on top</t>
+  </si>
+  <si>
+    <t>Shrimp, crab meat, cucumber, lettuce, spicy mayo, and masago</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Spicy Shrimp</t>
+  </si>
+  <si>
+    <t>Volcano</t>
+  </si>
+  <si>
+    <t>Spicy yellowtail, spicy tuna, and spicy salmon inside with masago</t>
+  </si>
+  <si>
+    <t>Crab, crunch, masago and mayo</t>
+  </si>
+  <si>
+    <t>Crab, spicy mayo, and crunch</t>
+  </si>
+  <si>
+    <t>Avocado, cucumber, crab, egg, pickled radish, and masago</t>
+  </si>
+  <si>
+    <t>Black &amp; White</t>
+  </si>
+  <si>
+    <t>Pop Up</t>
+  </si>
+  <si>
+    <t>Spicy tuna, crab, shrimp, cucumber, and avocado topped with masago and crunch</t>
+  </si>
+  <si>
+    <t>Dancing Tuna</t>
+  </si>
+  <si>
+    <t>Soft shell crab and cucumber topped with tuna</t>
+  </si>
+  <si>
+    <t>Fried roll with jalapeños, salmon, spicy crab, and honey cheese</t>
+  </si>
+  <si>
+    <t>Spicy salmon, cucumber, and crunch with salmon on top</t>
+  </si>
+  <si>
+    <t>St. Charles</t>
+  </si>
+  <si>
+    <t>Fried roll with red snapper, green onions, and cream cheese</t>
+  </si>
+  <si>
+    <t>Shrimp tempura and crab meat topped with honey cheese</t>
+  </si>
+  <si>
+    <t>Crazy Salmon</t>
+  </si>
+  <si>
+    <t>Fried salmon, and avocado toiled with spicy salon</t>
+  </si>
+  <si>
+    <t>Angry Dragon</t>
+  </si>
+  <si>
+    <t>Snow White</t>
+  </si>
+  <si>
+    <t>Fried crab meat and cucumber topped with honey cheese</t>
+  </si>
+  <si>
+    <t>Geisha</t>
+  </si>
+  <si>
+    <t>Fried fish and cucumber topped with crab meat</t>
+  </si>
+  <si>
+    <t>Shrimp tempura, cucumber, and avocado topped with crunch</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Green Tea</t>
+  </si>
+  <si>
+    <t>Red Bean</t>
   </si>
 </sst>
 </file>
@@ -977,6 +1366,14 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -6806,7 +7203,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="7.71"/>
     <col customWidth="1" min="2" max="2" width="22.0"/>
-    <col customWidth="1" min="3" max="3" width="45.29"/>
+    <col customWidth="1" min="3" max="3" width="14.14"/>
+    <col customWidth="1" min="4" max="4" width="45.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6816,7 +7214,10 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6827,6 +7228,9 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
@@ -6835,6 +7239,9 @@
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
@@ -6843,8 +7250,11 @@
       <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>291</v>
+      <c r="C4" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="5">
@@ -6854,6 +7264,9 @@
       <c r="B5" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
@@ -6865,6 +7278,9 @@
       <c r="C6" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="D6" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
@@ -6873,8 +7289,11 @@
       <c r="B7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>293</v>
+      <c r="C7" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="8">
@@ -6885,7 +7304,10 @@
         <v>165</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="9">
@@ -6898,6 +7320,9 @@
       <c r="C9" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
@@ -6909,6 +7334,9 @@
       <c r="C10" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="D10" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
@@ -6917,6 +7345,9 @@
       <c r="B11" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="C11" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
@@ -6925,6 +7356,9 @@
       <c r="B12" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
@@ -6933,8 +7367,11 @@
       <c r="B13" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>295</v>
+      <c r="C13" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="14">
@@ -6944,6 +7381,9 @@
       <c r="B14" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
@@ -6952,8 +7392,11 @@
       <c r="B15" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>296</v>
+      <c r="C15" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="16">
@@ -6963,6 +7406,9 @@
       <c r="B16" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="C16" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
@@ -6971,8 +7417,11 @@
       <c r="B17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>297</v>
+      <c r="C17" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="18">
@@ -6982,6 +7431,9 @@
       <c r="B18" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="C18" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
@@ -6989,6 +7441,2234 @@
       </c>
       <c r="B19" s="1" t="s">
         <v>264</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="7.86"/>
+    <col customWidth="1" min="2" max="2" width="20.29"/>
+    <col customWidth="1" min="3" max="3" width="22.86"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1">
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.0"/>
+    <col customWidth="1" min="2" max="2" width="20.14"/>
+    <col customWidth="1" min="3" max="3" width="24.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1">
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1">
+        <v>57.0</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1">
+        <v>58.0</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1">
+        <v>59.0</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1">
+        <v>61.0</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1">
+        <v>63.0</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1">
+        <v>66.0</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1">
+        <v>67.0</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1">
+        <v>68.0</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1">
+        <v>69.0</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1">
+        <v>71.0</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1">
+        <v>72.0</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1">
+        <v>73.0</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1">
+        <v>74.0</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1">
+        <v>76.0</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1">
+        <v>77.0</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1">
+        <v>78.0</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1">
+        <v>79.0</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1">
+        <v>81.0</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1">
+        <v>82.0</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1">
+        <v>83.0</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1">
+        <v>84.0</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1">
+        <v>86.0</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1">
+        <v>87.0</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1">
+        <v>88.0</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1">
+        <v>89.0</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1">
+        <v>91.0</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1">
+        <v>92.0</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1">
+        <v>93.0</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1">
+        <v>94.0</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1">
+        <v>96.0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>